<commit_message>
Result files from article
</commit_message>
<xml_diff>
--- a/quant_keys.xlsx
+++ b/quant_keys.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -425,41 +425,41 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>tratamientos homeopáticos</t>
+          <t>homeopatía</t>
         </is>
       </c>
       <c r="B1" t="n">
-        <v>2</v>
+        <v>460</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>homeopatia</t>
+          <t>homeópata</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>418</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>homeopatía</t>
+          <t>homeopatia</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>547</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>homeópata</t>
+          <t>tratamientos homeopáticos</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5">
@@ -469,27 +469,27 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>productos homeopáticos</t>
+          <t>medicina homeopática</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>medicina homeopática</t>
+          <t>miasmas</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8">
@@ -499,36 +499,76 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>miasmas</t>
+          <t>productos homeopáticos</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>memoria del agua</t>
+          <t>ley de los similares</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ley de los similares</t>
+          <t>memoria del agua</t>
         </is>
       </c>
       <c r="B11" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>ley de los infinitesimales</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>medicina homeopatica</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>homeopathic materia medica</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>remedios homeopaticos</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
         <v>1</v>
       </c>
     </row>
@@ -543,7 +583,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -554,170 +594,1636 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ser</t>
+          <t>Jornal de Notícias</t>
         </is>
       </c>
       <c r="B1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>homeopatía</t>
+          <t>JN</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>funcionar</t>
+          <t>Mundo</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ministerio de sanidad</t>
+          <t>medicamentos</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>estar</t>
+          <t>saúde</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>presentar</t>
+          <t>Espanha</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>orden</t>
+          <t>homeopatÃ­a</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ministerial</t>
+          <t>homeopatia</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>regular</t>
+          <t>pruebas</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>comercialización</t>
+          <t>efecto</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>país</t>
+          <t>placebo</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Jornal de Notícias</t>
+          <t>medicina</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>JN</t>
+          <t>alternativa</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Mundo</t>
+          <t>Hahnemann</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>medicamentos</t>
+          <t>ciencia</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>saúde</t>
+          <t>pseudociencia</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Espanha</t>
+          <t>pseudomedicina</t>
         </is>
       </c>
       <c r="B17" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>disoluciÃ³n</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>salud</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>doble</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>ciego</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>ensayo</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>ser</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>homeopatía</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>funcionar</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>ministerio de sanidad</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>estar</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>presentar</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>orden</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>ministerial</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>regular</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>comercialización</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>país</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Biblioteca Nacional de España</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Linked Data</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Datos enlazados</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Open Data</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Datos abiertos</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>cultura</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>cultura heritage</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>patrimonio cultural</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>libros</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>digitalizaciones</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>videos</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>mapas</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Homeopatía - Página de voz - Gran Enciclopedia Aragonesa OnLine Gran Enciclopedia Aragonesa Online</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Magento</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Varien</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>E-commerce</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>boiron</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>laboratorios</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>homoeopathy</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>homeopathy</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>homoeopathy for</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>homoeopathy books</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr"/>
+      <c r="B56" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>best homoeopathy website</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>most popular homoeopathy website</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>number one homoeopathy site</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>best homeopathy colleges india</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>free homoeopathy medical books</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>homeopathy india</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>homeo doctor</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>homeopathy courses</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>medical powerpoint prsentations</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>homeopathy powerpoints</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>research in homeopathy</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>online homeopathy consultation</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>jobs in homoeopathy</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>scope of homoeopathy</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>homoeopath medical news</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>homoeopathy treatment</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>homoeopathy news</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>homeopathic medicine</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>homoeopathic remedies</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>materia medica</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>job after bhms</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>homoeopathy teaching job</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>homoeopathy training</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>bhms</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>md(hom)</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>phd homoeopathy</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>homoeopathy repertory</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>homoeopathy apps</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>homoeopathy softwares</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>moh(uae) homoeopathy</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>pg courses after bhms</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>nrhm homeopathy job</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>dr mansoor ali</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>how to setup a clinic</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>question papers in homoeopathy</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>career in homoeopathy</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>best pg colleges in homoeopathy</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>psc upsc homoeopathy</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>cured cases in homoeopathy</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>best homeopathy doctor</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>moh uae question papers</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>psc upsc previous question papers</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>organon of medicine</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>homoeopathy job dubai</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>homoeopathy australia</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>history of homoeopathy india</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>scope of homoeopathy usa</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>homoeopathy in qatar</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>homoeopathy in bahrain</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>homoeopathy in saudi arabia</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>homoeopathy in oman</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>homoeopathy in pakistan</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>homoeopathy in malysia</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>homeopathy in europe</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>homoeopathy kerala</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>clinical tips in homoeopathy</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>placement after bhms</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>seminar in homeopathy</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>cme in homoeopathy</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>veterinary homoeopathy</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>health related courses after bhms</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>iec bcc in homoeopathy</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>kerala govt orders in homoeopathy</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>best pg homoeopathy colleges in india</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>latest news in homoeopathy</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>best homoeopathy treatment</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>study materials in homoeopathy</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>veterinary homeopathy courses</t>
+        </is>
+      </c>
+      <c r="B124" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>homoeopathy for pets</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Homeopatía</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>homeopatia si</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Boiron</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Medicamentos homeopaticos</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>cursos</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>curso online</t>
+        </is>
+      </c>
+      <c r="B131" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>cursos online</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>medico homeopata</t>
+        </is>
+      </c>
+      <c r="B133" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>homeopatia medicos</t>
+        </is>
+      </c>
+      <c r="B134" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>medicina homeopatia</t>
+        </is>
+      </c>
+      <c r="B135" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>medicos homeopatia</t>
+        </is>
+      </c>
+      <c r="B136" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>homeopatía madrid</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>médicos homeópatas</t>
+        </is>
+      </c>
+      <c r="B138" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>medicos homeopaticos</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>medico homeopata madrid</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>formación en homeopatía</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>curso de homeopatía para medicos</t>
+        </is>
+      </c>
+      <c r="B142" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>curso para medicos</t>
+        </is>
+      </c>
+      <c r="B143" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>terapéutica homeopática</t>
+        </is>
+      </c>
+      <c r="B144" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Iniciación médicos</t>
+        </is>
+      </c>
+      <c r="B145" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>experto médicos</t>
+        </is>
+      </c>
+      <c r="B146" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>perfeccionamiento médicos</t>
+        </is>
+      </c>
+      <c r="B147" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>talleres de homeopatía</t>
+        </is>
+      </c>
+      <c r="B148" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>seminarios homeopatía</t>
+        </is>
+      </c>
+      <c r="B149" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>terapéutica</t>
+        </is>
+      </c>
+      <c r="B150" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>homeopática</t>
+        </is>
+      </c>
+      <c r="B151" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>medicina de familia y homeopatía</t>
+        </is>
+      </c>
+      <c r="B152" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>formación continuada en homeopatía</t>
+        </is>
+      </c>
+      <c r="B153" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>vídeo</t>
+        </is>
+      </c>
+      <c r="B154" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>compartilhamento</t>
+        </is>
+      </c>
+      <c r="B155" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>celular com câmera</t>
+        </is>
+      </c>
+      <c r="B156" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>videofone</t>
+        </is>
+      </c>
+      <c r="B157" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>gratuito</t>
+        </is>
+      </c>
+      <c r="B158" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>envio</t>
+        </is>
+      </c>
+      <c r="B159" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>homeopatía homeopatia laboratorio homeopático boiron laboratorios medicamentos homeopáticos</t>
+        </is>
+      </c>
+      <c r="B160" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>BOIRON ESP</t>
+        </is>
+      </c>
+      <c r="B161" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>Podcast con H</t>
+        </is>
+      </c>
+      <c r="B162" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>medicamentos holísticos</t>
+        </is>
+      </c>
+      <c r="B163" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>medicamentos holisticos</t>
+        </is>
+      </c>
+      <c r="B164" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>